<commit_message>
removed extra art classes
</commit_message>
<xml_diff>
--- a/Resources/real_data/Input1_Refactored.xlsx
+++ b/Resources/real_data/Input1_Refactored.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="106">
   <si>
     <t>Course Name</t>
   </si>
@@ -831,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56:XFD56"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1308,9 +1308,6 @@
       <c r="F28" t="s">
         <v>48</v>
       </c>
-      <c r="I28" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
@@ -1809,9 +1806,6 @@
       <c r="G58" t="s">
         <v>66</v>
       </c>
-      <c r="I58" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="1" t="s">
@@ -1825,9 +1819,6 @@
       </c>
       <c r="G59" t="s">
         <v>66</v>
-      </c>
-      <c r="I59" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:9">

</xml_diff>